<commit_message>
Add instant bonito flakes and instant wine
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="395">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -978,6 +978,498 @@
 需要启用“启用自动倾倒”或“启用自动睡眠”。
 水和容器必须彼此靠近。</t>
   </si>
+  <si>
+    <t xml:space="preserve">title16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instant Bonito Flakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">即席かつお節</t>
+  </si>
+  <si>
+    <t xml:space="preserve">即时柴鱼片</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Instant Bonito Flakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">即席かつお節を有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用即时柴鱼片</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable instantly turning selected fish into bonito flakes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">選択した魚を即座にかつお節に変換する機能を有効または無効にします。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用将选定鱼类即时转化为柴鱼片。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instant Wine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">即席ワイン</t>
+  </si>
+  <si>
+    <t xml:space="preserve">即时酒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Instant Wine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">即席ワインを有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用即时酒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable instantly turning all fish items into wine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すべての魚アイテムを即座にワインに変換する機能を有効または無効にします。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用将所有鱼类物品即时转化为葡萄酒。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Fish for Bonito Flakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かつお節用の魚を選択</t>
+  </si>
+  <si>
+    <t xml:space="preserve">选择用于木鱼花的鱼 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ancient Fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">古代魚</t>
+  </si>
+  <si>
+    <t xml:space="preserve">古代鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arowana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">アロワナ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">龙鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スズキ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鲈鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitterling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゼニタナゴ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">田螺鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Bass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ブラックバス</t>
+  </si>
+  <si>
+    <t xml:space="preserve">黑鲈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blowfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">フグ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河豚</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">カツオ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鲣鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">コイ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鲤鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coelacanth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">シーラカンス</t>
+  </si>
+  <si>
+    <t xml:space="preserve">腔棘鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep Sea Fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">深海魚</t>
+  </si>
+  <si>
+    <t xml:space="preserve">深海鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ウナギ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鳗鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flatfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ヒラメ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">比目鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ハゼ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">虾虎鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goldfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金魚</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mackerel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">サバ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鲭鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moonfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ムーンフィッシュ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">月鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muddler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">カジカ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河鲇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Bream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">キンメダイ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">红鲷鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">サケ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三文鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sand Borer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">キス</t>
+  </si>
+  <si>
+    <t xml:space="preserve">沙钻鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sardine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">イワシ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">沙丁鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">キレアジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">竹荚鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea Bream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">マダイ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">真鲷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea Urchin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ウニ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海胆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">サメ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鲨鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Striped Jack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">シマアジ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">条纹鰺</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">マンボウ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">翻车鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweetfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">アユ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tadpole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おたまじゃくし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蝌蚪</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tilefish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">シロアマダイ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瓦鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuna 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ハリマグロ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">黄鳍金枪鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuna 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">マグロ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金枪鱼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turtle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">亀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海龟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">クジラ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鲸鱼</t>
+  </si>
 </sst>
 </file>
 
@@ -986,7 +1478,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1013,6 +1505,16 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1057,7 +1559,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1076,6 +1578,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1201,10 +1711,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2028,6 +2538,682 @@
         <v>230</v>
       </c>
     </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E67" s="1" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E68" s="1" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E69" s="1" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="E70" s="1" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E71" s="1" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E72" s="1" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E73" s="1" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E82" s="1" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="E83" s="1" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E84" s="1" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E85" s="1" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E86" s="1" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E87" s="1" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E88" s="1" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E89" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="E90" s="1" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E91" s="1" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E92" s="1" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="E93" s="1" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="E94" s="1" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="E95" s="1" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="E96" s="1" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="E97" s="1" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="E98" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="E99" s="1" t="n">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add instant read ancient books feature
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="407">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1470,6 +1470,42 @@
   <si>
     <t xml:space="preserve">鲸鱼</t>
   </si>
+  <si>
+    <t xml:space="preserve">title19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instant Read Ancient Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">インスタント古文書読書</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瞬间阅读古文书</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Instant Read Ancient Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">インスタント古文書読書を有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用瞬间阅读古文书</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable instant reading of ancient books.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">古文書を瞬時に読む機能を有効または無効にします。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用瞬间阅读古文书的功能。</t>
+  </si>
 </sst>
 </file>
 
@@ -1478,7 +1514,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1509,11 +1545,6 @@
     <font>
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1559,7 +1590,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1581,10 +1612,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1711,10 +1738,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1754,7 +1781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1768,7 +1795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1782,7 +1809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1796,7 +1823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1810,7 +1837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1824,7 +1851,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1838,7 +1865,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1866,7 +1893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1880,7 +1907,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -1894,7 +1921,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1908,7 +1935,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
@@ -1922,7 +1949,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1950,7 +1977,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -1964,7 +1991,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>67</v>
       </c>
@@ -1978,7 +2005,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -1992,7 +2019,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
@@ -2020,7 +2047,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>83</v>
       </c>
@@ -2034,7 +2061,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>87</v>
       </c>
@@ -2048,7 +2075,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>91</v>
       </c>
@@ -2062,7 +2089,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>95</v>
       </c>
@@ -2076,7 +2103,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
@@ -2104,7 +2131,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>107</v>
       </c>
@@ -2118,7 +2145,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>111</v>
       </c>
@@ -2132,7 +2159,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -2146,7 +2173,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>119</v>
       </c>
@@ -2160,7 +2187,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
@@ -2174,7 +2201,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>127</v>
       </c>
@@ -2188,7 +2215,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>131</v>
       </c>
@@ -2202,7 +2229,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>135</v>
       </c>
@@ -2216,7 +2243,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>139</v>
       </c>
@@ -2230,7 +2257,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>143</v>
       </c>
@@ -2244,7 +2271,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>147</v>
       </c>
@@ -2258,7 +2285,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>151</v>
       </c>
@@ -2286,7 +2313,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>159</v>
       </c>
@@ -2300,7 +2327,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>163</v>
       </c>
@@ -2314,7 +2341,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>167</v>
       </c>
@@ -2328,7 +2355,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>171</v>
       </c>
@@ -2342,7 +2369,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>175</v>
       </c>
@@ -2356,7 +2383,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>179</v>
       </c>
@@ -2370,7 +2397,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>183</v>
       </c>
@@ -2384,7 +2411,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>187</v>
       </c>
@@ -2412,7 +2439,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>195</v>
       </c>
@@ -2426,7 +2453,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>199</v>
       </c>
@@ -2440,7 +2467,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>203</v>
       </c>
@@ -2454,7 +2481,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>207</v>
       </c>
@@ -2468,7 +2495,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>211</v>
       </c>
@@ -2496,7 +2523,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>219</v>
       </c>
@@ -2510,7 +2537,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>223</v>
       </c>
@@ -2538,31 +2565,31 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>235</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="3" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2573,38 +2600,38 @@
       <c r="B61" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>247</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="3" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2615,28 +2642,28 @@
       <c r="B64" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>255</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>259</v>
       </c>
@@ -2646,14 +2673,14 @@
       <c r="C66" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="3" t="s">
         <v>262</v>
       </c>
       <c r="E66" s="1" t="n">
         <v>92</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>263</v>
       </c>
@@ -2663,14 +2690,14 @@
       <c r="C67" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="3" t="s">
         <v>266</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>74</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>267</v>
       </c>
@@ -2680,14 +2707,14 @@
       <c r="C68" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="3" t="s">
         <v>270</v>
       </c>
       <c r="E68" s="1" t="n">
         <v>69</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>271</v>
       </c>
@@ -2697,14 +2724,14 @@
       <c r="C69" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="3" t="s">
         <v>274</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>62</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>275</v>
       </c>
@@ -2714,14 +2741,14 @@
       <c r="C70" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="3" t="s">
         <v>278</v>
       </c>
       <c r="E70" s="1" t="n">
         <v>77</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>279</v>
       </c>
@@ -2731,14 +2758,14 @@
       <c r="C71" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="3" t="s">
         <v>282</v>
       </c>
       <c r="E71" s="1" t="n">
         <v>83</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>283</v>
       </c>
@@ -2748,14 +2775,14 @@
       <c r="C72" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="3" t="s">
         <v>286</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>81</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>287</v>
       </c>
@@ -2765,14 +2792,14 @@
       <c r="C73" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="3" t="s">
         <v>290</v>
       </c>
       <c r="E73" s="1" t="n">
         <v>65</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>291</v>
       </c>
@@ -2782,14 +2809,14 @@
       <c r="C74" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="3" t="s">
         <v>294</v>
       </c>
       <c r="E74" s="1" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>295</v>
       </c>
@@ -2799,14 +2826,14 @@
       <c r="C75" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="3" t="s">
         <v>298</v>
       </c>
       <c r="E75" s="1" t="n">
         <v>91</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>299</v>
       </c>
@@ -2816,14 +2843,14 @@
       <c r="C76" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="3" t="s">
         <v>302</v>
       </c>
       <c r="E76" s="1" t="n">
         <v>66</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>303</v>
       </c>
@@ -2833,14 +2860,14 @@
       <c r="C77" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="3" t="s">
         <v>306</v>
       </c>
       <c r="E77" s="1" t="n">
         <v>84</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>307</v>
       </c>
@@ -2850,14 +2877,14 @@
       <c r="C78" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="3" t="s">
         <v>310</v>
       </c>
       <c r="E78" s="1" t="n">
         <v>67</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>311</v>
       </c>
@@ -2867,14 +2894,14 @@
       <c r="C79" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="3" t="s">
         <v>314</v>
       </c>
       <c r="E79" s="1" t="n">
         <v>64</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>315</v>
       </c>
@@ -2884,14 +2911,14 @@
       <c r="C80" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="3" t="s">
         <v>318</v>
       </c>
       <c r="E80" s="1" t="n">
         <v>78</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>319</v>
       </c>
@@ -2901,14 +2928,14 @@
       <c r="C81" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="3" t="s">
         <v>322</v>
       </c>
       <c r="E81" s="1" t="n">
         <v>95</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>323</v>
       </c>
@@ -2918,14 +2945,14 @@
       <c r="C82" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="3" t="s">
         <v>326</v>
       </c>
       <c r="E82" s="1" t="n">
         <v>68</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>327</v>
       </c>
@@ -2935,14 +2962,14 @@
       <c r="C83" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="3" t="s">
         <v>330</v>
       </c>
       <c r="E83" s="1" t="n">
         <v>79</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>331</v>
       </c>
@@ -2952,14 +2979,14 @@
       <c r="C84" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E84" s="1" t="n">
         <v>87</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>335</v>
       </c>
@@ -2969,14 +2996,14 @@
       <c r="C85" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="3" t="s">
         <v>338</v>
       </c>
       <c r="E85" s="1" t="n">
         <v>88</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>339</v>
       </c>
@@ -2986,14 +3013,14 @@
       <c r="C86" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="3" t="s">
         <v>342</v>
       </c>
       <c r="E86" s="1" t="n">
         <v>85</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>343</v>
       </c>
@@ -3003,14 +3030,14 @@
       <c r="C87" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="3" t="s">
         <v>346</v>
       </c>
       <c r="E87" s="1" t="n">
         <v>72</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>347</v>
       </c>
@@ -3020,14 +3047,14 @@
       <c r="C88" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="3" t="s">
         <v>350</v>
       </c>
       <c r="E88" s="1" t="n">
         <v>86</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>351</v>
       </c>
@@ -3037,14 +3064,14 @@
       <c r="C89" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="3" t="s">
         <v>354</v>
       </c>
       <c r="E89" s="1" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>355</v>
       </c>
@@ -3054,14 +3081,14 @@
       <c r="C90" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="3" t="s">
         <v>358</v>
       </c>
       <c r="E90" s="1" t="n">
         <v>93</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>359</v>
       </c>
@@ -3071,14 +3098,14 @@
       <c r="C91" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="3" t="s">
         <v>362</v>
       </c>
       <c r="E91" s="1" t="n">
         <v>76</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>363</v>
       </c>
@@ -3088,14 +3115,14 @@
       <c r="C92" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="3" t="s">
         <v>366</v>
       </c>
       <c r="E92" s="1" t="n">
         <v>94</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>367</v>
       </c>
@@ -3105,14 +3132,14 @@
       <c r="C93" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="3" t="s">
         <v>370</v>
       </c>
       <c r="E93" s="1" t="n">
         <v>75</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>371</v>
       </c>
@@ -3122,14 +3149,14 @@
       <c r="C94" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="3" t="s">
         <v>374</v>
       </c>
       <c r="E94" s="1" t="n">
         <v>63</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>375</v>
       </c>
@@ -3139,14 +3166,14 @@
       <c r="C95" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="3" t="s">
         <v>378</v>
       </c>
       <c r="E95" s="1" t="n">
         <v>71</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>379</v>
       </c>
@@ -3156,14 +3183,14 @@
       <c r="C96" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="3" t="s">
         <v>382</v>
       </c>
       <c r="E96" s="1" t="n">
         <v>73</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>383</v>
       </c>
@@ -3173,14 +3200,14 @@
       <c r="C97" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="3" t="s">
         <v>386</v>
       </c>
       <c r="E97" s="1" t="n">
         <v>82</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>387</v>
       </c>
@@ -3190,14 +3217,14 @@
       <c r="C98" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="3" t="s">
         <v>390</v>
       </c>
       <c r="E98" s="1" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>391</v>
       </c>
@@ -3207,11 +3234,53 @@
       <c r="C99" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="3" t="s">
         <v>394</v>
       </c>
       <c r="E99" s="1" t="n">
         <v>89</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix nearest fishing point
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -1514,7 +1514,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1541,11 +1541,6 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1590,7 +1585,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1609,10 +1604,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1740,8 +1731,8 @@
   </sheetPr>
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B117" activeCellId="0" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1750,7 +1741,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="65.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="65.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="67.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="6" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,6 +1939,7 @@
       <c r="D14" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="E14" s="0"/>
     </row>
     <row r="15" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -1962,6 +1954,7 @@
       <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="E15" s="0"/>
     </row>
     <row r="16" s="4" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -1976,6 +1969,7 @@
       <c r="D16" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E16" s="0"/>
     </row>
     <row r="17" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -1990,6 +1984,7 @@
       <c r="D17" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="E17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -2659,7 +2654,7 @@
       <c r="C65" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="3" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2676,9 +2671,6 @@
       <c r="D66" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E66" s="1" t="n">
-        <v>92</v>
-      </c>
     </row>
     <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
@@ -2693,9 +2685,6 @@
       <c r="D67" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E67" s="1" t="n">
-        <v>74</v>
-      </c>
     </row>
     <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
@@ -2710,9 +2699,6 @@
       <c r="D68" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E68" s="1" t="n">
-        <v>69</v>
-      </c>
     </row>
     <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -2727,9 +2713,6 @@
       <c r="D69" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E69" s="1" t="n">
-        <v>62</v>
-      </c>
     </row>
     <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
@@ -2744,9 +2727,6 @@
       <c r="D70" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="E70" s="1" t="n">
-        <v>77</v>
-      </c>
     </row>
     <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
@@ -2761,9 +2741,6 @@
       <c r="D71" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="E71" s="1" t="n">
-        <v>83</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
@@ -2778,9 +2755,6 @@
       <c r="D72" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E72" s="1" t="n">
-        <v>81</v>
-      </c>
     </row>
     <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
@@ -2795,9 +2769,6 @@
       <c r="D73" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="E73" s="1" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
@@ -2812,9 +2783,6 @@
       <c r="D74" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="E74" s="1" t="n">
-        <v>90</v>
-      </c>
     </row>
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
@@ -2829,9 +2797,6 @@
       <c r="D75" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E75" s="1" t="n">
-        <v>91</v>
-      </c>
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
@@ -2846,9 +2811,6 @@
       <c r="D76" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E76" s="1" t="n">
-        <v>66</v>
-      </c>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
@@ -2863,9 +2825,6 @@
       <c r="D77" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E77" s="1" t="n">
-        <v>84</v>
-      </c>
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
@@ -2880,9 +2839,6 @@
       <c r="D78" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="E78" s="1" t="n">
-        <v>67</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
@@ -2897,9 +2853,6 @@
       <c r="D79" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E79" s="1" t="n">
-        <v>64</v>
-      </c>
     </row>
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
@@ -2914,9 +2867,6 @@
       <c r="D80" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="E80" s="1" t="n">
-        <v>78</v>
-      </c>
     </row>
     <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
@@ -2931,9 +2881,6 @@
       <c r="D81" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E81" s="1" t="n">
-        <v>95</v>
-      </c>
     </row>
     <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
@@ -2948,9 +2895,6 @@
       <c r="D82" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E82" s="1" t="n">
-        <v>68</v>
-      </c>
     </row>
     <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
@@ -2965,9 +2909,6 @@
       <c r="D83" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E83" s="1" t="n">
-        <v>79</v>
-      </c>
     </row>
     <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
@@ -2982,9 +2923,6 @@
       <c r="D84" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="E84" s="1" t="n">
-        <v>87</v>
-      </c>
     </row>
     <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
@@ -2999,9 +2937,6 @@
       <c r="D85" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="E85" s="1" t="n">
-        <v>88</v>
-      </c>
     </row>
     <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
@@ -3016,9 +2951,6 @@
       <c r="D86" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="E86" s="1" t="n">
-        <v>85</v>
-      </c>
     </row>
     <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
@@ -3033,9 +2965,6 @@
       <c r="D87" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="E87" s="1" t="n">
-        <v>72</v>
-      </c>
     </row>
     <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
@@ -3050,9 +2979,6 @@
       <c r="D88" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="E88" s="1" t="n">
-        <v>86</v>
-      </c>
     </row>
     <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
@@ -3067,9 +2993,6 @@
       <c r="D89" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="E89" s="1" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
@@ -3084,9 +3007,6 @@
       <c r="D90" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="E90" s="1" t="n">
-        <v>93</v>
-      </c>
     </row>
     <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
@@ -3101,9 +3021,6 @@
       <c r="D91" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="E91" s="1" t="n">
-        <v>76</v>
-      </c>
     </row>
     <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
@@ -3118,9 +3035,6 @@
       <c r="D92" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="E92" s="1" t="n">
-        <v>94</v>
-      </c>
     </row>
     <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
@@ -3135,9 +3049,6 @@
       <c r="D93" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="E93" s="1" t="n">
-        <v>75</v>
-      </c>
     </row>
     <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
@@ -3152,9 +3063,6 @@
       <c r="D94" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="E94" s="1" t="n">
-        <v>63</v>
-      </c>
     </row>
     <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
@@ -3169,9 +3077,6 @@
       <c r="D95" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="E95" s="1" t="n">
-        <v>71</v>
-      </c>
     </row>
     <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
@@ -3186,9 +3091,6 @@
       <c r="D96" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="E96" s="1" t="n">
-        <v>73</v>
-      </c>
     </row>
     <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
@@ -3203,9 +3105,6 @@
       <c r="D97" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="E97" s="1" t="n">
-        <v>82</v>
-      </c>
     </row>
     <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
@@ -3220,9 +3119,6 @@
       <c r="D98" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="E98" s="1" t="n">
-        <v>80</v>
-      </c>
     </row>
     <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
@@ -3237,9 +3133,6 @@
       <c r="D99" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="E99" s="1" t="n">
-        <v>89</v>
-      </c>
     </row>
     <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
@@ -3248,10 +3141,10 @@
       <c r="B100" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="3" t="s">
         <v>398</v>
       </c>
     </row>
@@ -3262,10 +3155,10 @@
       <c r="B101" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="3" t="s">
         <v>402</v>
       </c>
     </row>
@@ -3276,10 +3169,10 @@
       <c r="B102" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="3" t="s">
         <v>406</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add exclude tier fish
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="415">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -997,10 +997,10 @@
     <t xml:space="preserve">Enable Instant Bonito Flakes</t>
   </si>
   <si>
-    <t xml:space="preserve">即席かつお節を有効化</t>
-  </si>
-  <si>
-    <t xml:space="preserve">启用即时柴鱼片</t>
+    <t xml:space="preserve">かつおぶし変換を即座に有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用即时柴鱼片转换</t>
   </si>
   <si>
     <t xml:space="preserve">tooltip16</t>
@@ -1009,7 +1009,7 @@
     <t xml:space="preserve">Enable or disable instantly turning selected fish into bonito flakes.</t>
   </si>
   <si>
-    <t xml:space="preserve">選択した魚を即座にかつお節に変換する機能を有効または無効にします。</t>
+    <t xml:space="preserve">選択した魚をかつおぶしに即座に変換する機能を有効または無効にします。</t>
   </si>
   <si>
     <t xml:space="preserve">启用或禁用将选定鱼类即时转化为柴鱼片。</t>
@@ -1505,6 +1505,81 @@
   </si>
   <si>
     <t xml:space="preserve">启用或禁用瞬间阅读古文书的功能。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Exclude Tier Fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">星付き魚を除外</t>
+  </si>
+  <si>
+    <t xml:space="preserve">排除星级鱼类</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable excluding star-tier (★) fish from the bonito flakes feature.
+Set to 'true' to skip converting rare fish marked with a star.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">星付き（★）のレア魚をかつおぶし変換機能の対象から除外するかどうかを設定します。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'true' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">に設定すると、★付きの魚は変換されません。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">启用或禁用将带有星标（★）的稀有鱼类排除在柴鱼片转换功能之外。
+设置为 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'true' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">可跳过转换带星的稀有鱼类。</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1514,7 +1589,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1541,6 +1616,11 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1585,7 +1665,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1604,6 +1684,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1729,10 +1813,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B117" activeCellId="0" sqref="B117"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D108" activeCellId="0" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1939,7 +2023,6 @@
       <c r="D14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="0"/>
     </row>
     <row r="15" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -1954,7 +2037,6 @@
       <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="0"/>
     </row>
     <row r="16" s="4" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -1969,7 +2051,6 @@
       <c r="D16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="0"/>
     </row>
     <row r="17" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -1984,7 +2065,6 @@
       <c r="D17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -3174,6 +3254,34 @@
       </c>
       <c r="D102" s="3" t="s">
         <v>406</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for EA 23.213 Stable. Added No Stamina Cost while fishing. Toggle it in the Config menu. Off by default.
EA 23.213 Stable に対応しました。
釣り中のスタミナ消費なしを追加しました。設定メニューから切り替え可能です。デフォルトは無効です。

已更新至 EA 23.213 Stable。
新增钓鱼时不消耗体力选项。可在设置菜单中切换。默认关闭。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="439">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1569,6 +1569,42 @@
   <si>
     <t xml:space="preserve">启用或禁用为钓到的鱼设置自定义星级（★）。</t>
   </si>
+  <si>
+    <t xml:space="preserve">title21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Stamina Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スタミナ消費なし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">不消耗体力</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable No Stamina Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スタミナ消費なしを有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用不消耗体力</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable no stamina cost while fishing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">釣り中のスタミナ消費なしを有効または無効にします。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用钓鱼时不消耗体力。</t>
+  </si>
 </sst>
 </file>
 
@@ -1577,7 +1613,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1610,11 +1646,6 @@
       <name val="Noto Sans SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1664,7 +1695,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1690,10 +1721,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1833,15 +1860,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D111" activeCellId="0" sqref="D111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C118" activeCellId="0" sqref="C118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="65.95"/>
@@ -2045,7 +2072,6 @@
       <c r="D14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="0"/>
     </row>
     <row r="15" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -2060,7 +2086,6 @@
       <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="0"/>
     </row>
     <row r="16" s="4" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -2075,7 +2100,6 @@
       <c r="D16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="0"/>
     </row>
     <row r="17" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -2090,7 +2114,6 @@
       <c r="D17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -2218,7 +2241,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -2400,7 +2423,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>155</v>
       </c>
@@ -2526,7 +2549,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>191</v>
       </c>
@@ -2736,7 +2759,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>251</v>
       </c>
@@ -3296,7 +3319,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>411</v>
       </c>
@@ -3310,7 +3333,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
         <v>415</v>
       </c>
@@ -3320,36 +3343,78 @@
       <c r="C105" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="D105" s="5" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>419</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C106" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="D106" s="5" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
         <v>423</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="D107" s="5" t="s">
         <v>426</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for EA 23.222 Stable. Added No Bait Consumption while fishing. Toggle it in the Config menu. Off by default.
EA 23.222 Stable に対応しました。
釣り中の餌消費なしを追加しました。設定メニューから切り替え可能です。デフォルトは無効です。

已更新至 EA 23.222 Stable。
新增钓鱼时不消耗鱼饵选项。可在设置菜单中切换。默认关闭。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="451">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1604,6 +1604,42 @@
   </si>
   <si>
     <t xml:space="preserve">启用或禁用钓鱼时不消耗体力。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Bait Consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">餌消費なし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">不消耗鱼饵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable No Bait Consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">餌消費なしを有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用不消耗鱼饵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable no bait consumption while fishing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">釣り中の餌消費なしを有効または無効にします。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用钓鱼时不消耗鱼饵。</t>
   </si>
 </sst>
 </file>
@@ -1860,12 +1896,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C118" activeCellId="0" sqref="C118"/>
+      <selection pane="bottomLeft" activeCell="C102" activeCellId="0" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3340,7 +3376,7 @@
       <c r="B105" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C105" s="6" t="s">
+      <c r="C105" s="5" t="s">
         <v>417</v>
       </c>
       <c r="D105" s="5" t="s">
@@ -3382,10 +3418,10 @@
       <c r="B108" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="C108" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="D108" s="6" t="s">
+      <c r="D108" s="5" t="s">
         <v>430</v>
       </c>
     </row>
@@ -3396,10 +3432,10 @@
       <c r="B109" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="C109" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="D109" s="6" t="s">
+      <c r="D109" s="5" t="s">
         <v>434</v>
       </c>
     </row>
@@ -3410,11 +3446,53 @@
       <c r="B110" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C110" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="D110" s="6" t="s">
+      <c r="D110" s="5" t="s">
         <v>438</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>